<commit_message>
feat: add avatar photo retrieve and fix some tests
</commit_message>
<xml_diff>
--- a/docs/Requirements.xlsx
+++ b/docs/Requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\felipe\Projects\tcc\helpcar-server\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\felipe\Projects\helpcar-server\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{567DC1CB-BC28-4F7E-BF28-D2285EC142D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF13319-69EC-4022-B5A7-2AA1327EA63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{9FDF1E00-D307-4BA6-A2BC-F1837E9A6378}"/>
   </bookViews>
@@ -156,7 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,11 +171,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -241,7 +236,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
@@ -249,7 +244,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -305,7 +300,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -313,7 +308,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -335,15 +330,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>611256</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>186941</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -399,14 +394,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
@@ -415,7 +415,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE691CF3-F5B3-4B36-807E-CAEB16259E2F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -455,20 +455,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
@@ -477,7 +482,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AB0571B-E99D-444C-AAA0-F61613B5929A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -517,20 +522,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
@@ -539,7 +549,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18C1CFD2-9954-4B41-9CFC-B5A98F6EAE24}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -579,20 +589,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1034" name="Check Box 10" hidden="1">
@@ -601,7 +616,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8214F421-2542-4FD2-821B-C66573A3C123}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -641,20 +656,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1035" name="Check Box 11" hidden="1">
@@ -663,7 +683,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A957DD88-58CD-4E13-9493-E61808C6A71F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -703,20 +723,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1036" name="Check Box 12" hidden="1">
@@ -725,7 +750,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA1EFE74-2771-4596-9924-2812A46BE81F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -765,20 +790,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
@@ -787,7 +817,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB1ABC94-B53A-4BB5-9380-F1BD8FC4355D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -827,20 +857,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
@@ -849,7 +884,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DB2C88C-FEEF-4171-9911-13FAE38C7125}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -889,20 +924,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
@@ -911,7 +951,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{003252DD-1CAF-4928-97C1-63C80695994E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -951,20 +991,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
@@ -973,7 +1018,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CCBAA52-25FF-4625-8A55-8D762D5C0D1D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1013,20 +1058,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
@@ -1035,7 +1085,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45064107-7FCE-4712-9CC9-EC05047C60F9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1075,20 +1125,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
@@ -1097,7 +1152,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4811E924-1319-4190-B0F4-B36846E1B814}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1137,20 +1192,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
@@ -1159,7 +1219,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{388FA389-4DBE-4257-AE13-2442C25F5867}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1199,20 +1259,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
@@ -1221,7 +1286,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3000A75B-9FE5-41A6-9E7B-179A665B7A1C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1261,20 +1326,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
@@ -1283,7 +1353,7 @@
                   <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EDE5F22-11BB-45A2-BDB7-582CBCF2773B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1323,20 +1393,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
@@ -1345,7 +1420,7 @@
                   <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B535A0F3-BFC6-453B-BDF6-070021C62008}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1385,20 +1460,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1048" name="Check Box 24" hidden="1">
@@ -1407,7 +1487,7 @@
                   <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{356D4EC9-1112-45B0-BE4B-6B8B913F6327}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1447,20 +1527,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1049" name="Check Box 25" hidden="1">
@@ -1469,7 +1554,7 @@
                   <a14:compatExt spid="_x0000_s1049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DAA07E2-427D-4743-B5DF-AD738550EC19}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1509,20 +1594,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
@@ -1531,7 +1621,7 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1CFC354-A0F5-4145-8B71-0C70EB88E5CA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1571,20 +1661,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1051" name="Check Box 27" hidden="1">
@@ -1593,7 +1688,7 @@
                   <a14:compatExt spid="_x0000_s1051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5350496-84DB-4C97-85EC-E6EA4C0B2043}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1633,20 +1728,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1052" name="Check Box 28" hidden="1">
@@ -1655,7 +1755,7 @@
                   <a14:compatExt spid="_x0000_s1052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB26D354-5ED3-4532-B9CF-D30A0625901D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1695,20 +1795,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>301137</xdr:colOff>
+          <xdr:colOff>304800</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>167891</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="310119" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1053" name="Check Box 29" hidden="1">
@@ -1717,7 +1822,7 @@
                   <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B90C006-B448-4D8B-B840-D3415AD04DD6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1757,7 +1862,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -2064,7 +2169,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,7 +2359,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>